<commit_message>
Changed Default names for activities
</commit_message>
<xml_diff>
--- a/SourceCode/2023/Sep2023/Projects/Sarath Chandra/REFWI5/ACME/WI5.xlsx
+++ b/SourceCode/2023/Sep2023/Projects/Sarath Chandra/REFWI5/ACME/WI5.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <x:si>
     <x:t>WIID</x:t>
   </x:si>
@@ -34,7 +34,7 @@
     <x:t>Date</x:t>
   </x:si>
   <x:si>
-    <x:t>95307830</x:t>
+    <x:t>95310357</x:t>
   </x:si>
   <x:si>
     <x:t>Calculate Client Security Hash</x:t>
@@ -46,103 +46,115 @@
     <x:t>Open</x:t>
   </x:si>
   <x:si>
-    <x:t>2017-09-30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95307835</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-08-13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95307828</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2021-01-03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305625</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2019-06-23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305623</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-02-01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305612</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-12-23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305626</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2020-08-10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305628</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2023-04-04</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305621</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2021-10-28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305616</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-10-26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305619</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2019-05-14</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305627</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-11-29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305618</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-04-15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305617</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2019-10-19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305614</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2023-04-30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305613</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-01-20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>95305622</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-04-21</x:t>
+    <x:t>2022-05-02</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310351</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2022-06-04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310347</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-04-07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310364</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2020-11-22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310362</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2020-07-21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310358</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2019-09-07</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310356</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-05-20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310348</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-08-12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310355</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-09-23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310363</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2023-07-29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310349</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2019-01-08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310352</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2023-03-20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310360</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2020-02-23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310346</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2019-04-08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310359</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2023-01-04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310361</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-04-16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310350</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-12-21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310354</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2019-11-28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>95310353</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2021-08-25</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -800,6 +812,40 @@
         <x:v>41</x:v>
       </x:c>
     </x:row>
+    <x:row r="19" spans="1:5">
+      <x:c r="A19" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:5">
+      <x:c r="A20" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>